<commit_message>
china ReEAP bar graph datawrapper
</commit_message>
<xml_diff>
--- a/new-version/data/dreaded-bar-anime-data-for-use.xlsx
+++ b/new-version/data/dreaded-bar-anime-data-for-use.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judyyang/GitHub/24f402c1-271d-4361-a6b3-2ad3a1fcffe1/new-version/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{71D773CD-4DFF-9446-A803-3DDA375CEF48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5410EC09-CD80-B54D-B0CD-008C8EEFC9EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Threshold</t>
   </si>
@@ -1135,7 +1135,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'dreaded-bar-anime-data-for-use'!$M$18</c:f>
+              <c:f>'dreaded-bar-anime-data-for-use'!$L$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1182,7 +1182,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'dreaded-bar-anime-data-for-use'!$M$19:$M$24</c:f>
+              <c:f>'dreaded-bar-anime-data-for-use'!$L$19:$L$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1218,7 +1218,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'dreaded-bar-anime-data-for-use'!$N$18</c:f>
+              <c:f>'dreaded-bar-anime-data-for-use'!$M$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1265,7 +1265,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'dreaded-bar-anime-data-for-use'!$N$19:$N$24</c:f>
+              <c:f>'dreaded-bar-anime-data-for-use'!$M$19:$M$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2594,15 +2594,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2629,16 +2629,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2968,7 +2968,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="K18" sqref="K18:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3705,10 +3705,7 @@
         <v>23.477212080000001</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -3718,20 +3715,17 @@
       <c r="D18" t="s">
         <v>11</v>
       </c>
+      <c r="K18" t="s">
+        <v>10</v>
+      </c>
       <c r="L18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="M18" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -3741,20 +3735,17 @@
       <c r="D19">
         <v>409.06788849999998</v>
       </c>
-      <c r="L19" t="s">
+      <c r="K19" t="s">
         <v>3</v>
       </c>
+      <c r="L19">
+        <v>27.99254711</v>
+      </c>
       <c r="M19">
-        <v>27.99254711</v>
-      </c>
-      <c r="N19">
         <v>6.080053961</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -3764,20 +3755,17 @@
       <c r="D20">
         <v>332.66783149999998</v>
       </c>
-      <c r="L20" t="s">
+      <c r="K20" t="s">
         <v>4</v>
       </c>
+      <c r="L20">
+        <v>100.0747392</v>
+      </c>
       <c r="M20">
-        <v>100.0747392</v>
-      </c>
-      <c r="N20">
         <v>57.736415119999997</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -3787,20 +3775,17 @@
       <c r="D21">
         <v>292.0252127</v>
       </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s">
         <v>5</v>
       </c>
+      <c r="L21">
+        <v>163.2077338</v>
+      </c>
       <c r="M21">
-        <v>163.2077338</v>
-      </c>
-      <c r="N21">
         <v>233.9518774</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -3810,20 +3795,17 @@
       <c r="D22">
         <v>227.26977719999999</v>
       </c>
-      <c r="L22" t="s">
+      <c r="K22" t="s">
         <v>6</v>
       </c>
+      <c r="L22">
+        <v>259.55610840000003</v>
+      </c>
       <c r="M22">
-        <v>259.55610840000003</v>
-      </c>
-      <c r="N22">
         <v>741.38426689999994</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -3833,20 +3815,17 @@
       <c r="D23">
         <v>18.680304249999999</v>
       </c>
-      <c r="L23" t="s">
+      <c r="K23" t="s">
         <v>7</v>
       </c>
+      <c r="L23">
+        <v>82.121707499999999</v>
+      </c>
       <c r="M23">
-        <v>82.121707499999999</v>
-      </c>
-      <c r="N23">
         <v>332.91519549999998</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -3856,13 +3835,13 @@
       <c r="D24">
         <v>0.68898580099999995</v>
       </c>
-      <c r="L24" t="s">
+      <c r="K24" t="s">
         <v>8</v>
       </c>
+      <c r="L24">
+        <v>23.477212080000001</v>
+      </c>
       <c r="M24">
-        <v>23.477212080000001</v>
-      </c>
-      <c r="N24">
         <v>14.327191150000001</v>
       </c>
     </row>

</xml_diff>